<commit_message>
added umd 23 troll files
</commit_message>
<xml_diff>
--- a/raw_data/umd/2023/RL_2023-06-01_MB5a.xlsx
+++ b/raw_data/umd/2023/RL_2023-06-01_MB5a.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\CSE\Llo\LAB-stern007\AQ400 Data files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samblackburn/Documents/lshabs/raw_data/umd/2023/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{04176ACD-6BEA-446D-BC3D-B0593D2390BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04675425-71E1-114F-A7BA-ED7596728294}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4965" yWindow="420" windowWidth="21495" windowHeight="13920" xr2:uid="{7D425A1C-8188-4CDD-A616-B6B07E7A0ED8}"/>
+    <workbookView xWindow="4960" yWindow="760" windowWidth="21500" windowHeight="13920" xr2:uid="{7D425A1C-8188-4CDD-A616-B6B07E7A0ED8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -151,9 +151,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -191,7 +191,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -297,7 +297,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -439,7 +439,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -447,121 +447,172 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4437D9F-5E91-4DCA-A0B3-57D464DDA792}">
-  <dimension ref="A1:R46"/>
+  <dimension ref="A1:R45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T7" sqref="T7"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" customWidth="1"/>
+    <col min="1" max="1" width="16.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A1" s="1"/>
-    </row>
-    <row r="2" spans="1:18" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+    <row r="1" spans="1:18" ht="75" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
+        <v>45098.533229166664</v>
+      </c>
+      <c r="B2" s="1">
+        <v>6.1880139999999999</v>
+      </c>
+      <c r="C2" s="1">
+        <v>9.7539650000000009</v>
+      </c>
+      <c r="D2" s="1">
+        <v>80.014080000000007</v>
+      </c>
+      <c r="E2" s="1">
+        <v>104.871</v>
+      </c>
+      <c r="F2" s="1">
+        <v>4.8908689999999998E-2</v>
+      </c>
+      <c r="G2" s="1">
+        <v>0.99946840000000003</v>
+      </c>
+      <c r="H2" s="1">
+        <v>6.797446E-2</v>
+      </c>
+      <c r="I2" s="1">
+        <v>1.165851</v>
+      </c>
+      <c r="J2" s="1">
+        <v>12.660629999999999</v>
+      </c>
+      <c r="K2" s="1">
+        <v>0.25052730000000001</v>
+      </c>
+      <c r="L2" s="1">
+        <v>1.2048099999999999</v>
+      </c>
+      <c r="M2" s="1">
+        <v>0.175705</v>
+      </c>
+      <c r="N2" s="1">
+        <v>16.833850000000002</v>
+      </c>
+      <c r="O2" s="1">
+        <v>999.4203</v>
+      </c>
+      <c r="P2" s="1">
+        <v>46.887215519999998</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>-91.050268259999996</v>
+      </c>
+      <c r="R2" s="1"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
-        <v>45098.533229166664</v>
+        <v>45098.53324074074</v>
       </c>
       <c r="B3" s="1">
-        <v>6.1880139999999999</v>
+        <v>6.1971100000000003</v>
       </c>
       <c r="C3" s="1">
-        <v>9.7539650000000009</v>
+        <v>9.7755220000000005</v>
       </c>
       <c r="D3" s="1">
-        <v>80.014080000000007</v>
+        <v>79.982590000000002</v>
       </c>
       <c r="E3" s="1">
-        <v>104.871</v>
+        <v>104.8527</v>
       </c>
       <c r="F3" s="1">
-        <v>4.8908689999999998E-2</v>
+        <v>4.8899320000000003E-2</v>
       </c>
       <c r="G3" s="1">
-        <v>0.99946840000000003</v>
+        <v>0.99946939999999995</v>
       </c>
       <c r="H3" s="1">
-        <v>6.797446E-2</v>
+        <v>6.7767250000000001E-2</v>
       </c>
       <c r="I3" s="1">
-        <v>1.165851</v>
+        <v>1.175047</v>
       </c>
       <c r="J3" s="1">
-        <v>12.660629999999999</v>
+        <v>12.65649</v>
       </c>
       <c r="K3" s="1">
-        <v>0.25052730000000001</v>
+        <v>0.25221719999999997</v>
       </c>
       <c r="L3" s="1">
-        <v>1.2048099999999999</v>
+        <v>1.207422</v>
       </c>
       <c r="M3" s="1">
-        <v>0.175705</v>
+        <v>0.17645169999999999</v>
       </c>
       <c r="N3" s="1">
-        <v>16.833850000000002</v>
+        <v>16.835740000000001</v>
       </c>
       <c r="O3" s="1">
-        <v>999.4203</v>
+        <v>999.42110000000002</v>
       </c>
       <c r="P3" s="1">
         <v>46.887215519999998</v>
@@ -573,49 +624,49 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
-        <v>45098.53324074074</v>
+        <v>45098.533252314817</v>
       </c>
       <c r="B4" s="1">
-        <v>6.1971100000000003</v>
+        <v>6.2099080000000004</v>
       </c>
       <c r="C4" s="1">
-        <v>9.7755220000000005</v>
+        <v>10.0945</v>
       </c>
       <c r="D4" s="1">
-        <v>79.982590000000002</v>
+        <v>80.594890000000007</v>
       </c>
       <c r="E4" s="1">
-        <v>104.8527</v>
+        <v>105.7924</v>
       </c>
       <c r="F4" s="1">
-        <v>4.8899320000000003E-2</v>
+        <v>4.9348940000000001E-2</v>
       </c>
       <c r="G4" s="1">
-        <v>0.99946939999999995</v>
+        <v>0.99947600000000003</v>
       </c>
       <c r="H4" s="1">
-        <v>6.7767250000000001E-2</v>
+        <v>6.8806080000000006E-2</v>
       </c>
       <c r="I4" s="1">
-        <v>1.175047</v>
+        <v>1.1587400000000001</v>
       </c>
       <c r="J4" s="1">
-        <v>12.65649</v>
+        <v>12.537039999999999</v>
       </c>
       <c r="K4" s="1">
-        <v>0.25221719999999997</v>
+        <v>0.25792140000000002</v>
       </c>
       <c r="L4" s="1">
-        <v>1.207422</v>
+        <v>1.222677</v>
       </c>
       <c r="M4" s="1">
-        <v>0.17645169999999999</v>
+        <v>0.18142939999999999</v>
       </c>
       <c r="N4" s="1">
-        <v>16.835740000000001</v>
+        <v>16.8</v>
       </c>
       <c r="O4" s="1">
-        <v>999.42110000000002</v>
+        <v>999.41070000000002</v>
       </c>
       <c r="P4" s="1">
         <v>46.887215519999998</v>
@@ -627,157 +678,157 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
-        <v>45098.533252314817</v>
+        <v>45098.533263888887</v>
       </c>
       <c r="B5" s="1">
-        <v>6.2099080000000004</v>
+        <v>6.2142660000000003</v>
       </c>
       <c r="C5" s="1">
-        <v>10.0945</v>
+        <v>10.119199999999999</v>
       </c>
       <c r="D5" s="1">
-        <v>80.594890000000007</v>
+        <v>80.612489999999994</v>
       </c>
       <c r="E5" s="1">
-        <v>105.7924</v>
+        <v>105.8317</v>
       </c>
       <c r="F5" s="1">
-        <v>4.9348940000000001E-2</v>
+        <v>4.9367479999999998E-2</v>
       </c>
       <c r="G5" s="1">
-        <v>0.99947600000000003</v>
+        <v>0.9994767</v>
       </c>
       <c r="H5" s="1">
-        <v>6.8806080000000006E-2</v>
+        <v>6.8773029999999999E-2</v>
       </c>
       <c r="I5" s="1">
-        <v>1.1587400000000001</v>
+        <v>1.1616899999999999</v>
       </c>
       <c r="J5" s="1">
-        <v>12.537039999999999</v>
+        <v>12.529400000000001</v>
       </c>
       <c r="K5" s="1">
-        <v>0.25792140000000002</v>
+        <v>0.25889659999999998</v>
       </c>
       <c r="L5" s="1">
-        <v>1.222677</v>
+        <v>1.224505</v>
       </c>
       <c r="M5" s="1">
-        <v>0.18142939999999999</v>
+        <v>0.18198259999999999</v>
       </c>
       <c r="N5" s="1">
-        <v>16.8</v>
+        <v>16.79899</v>
       </c>
       <c r="O5" s="1">
-        <v>999.41070000000002</v>
+        <v>999.41049999999996</v>
       </c>
       <c r="P5" s="1">
-        <v>46.887215519999998</v>
+        <v>46.887207119999999</v>
       </c>
       <c r="Q5" s="1">
-        <v>-91.050268259999996</v>
+        <v>-91.050254019999997</v>
       </c>
       <c r="R5" s="1"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
-        <v>45098.533263888887</v>
+        <v>45098.533275462964</v>
       </c>
       <c r="B6" s="1">
-        <v>6.2142660000000003</v>
+        <v>6.2186240000000002</v>
       </c>
       <c r="C6" s="1">
-        <v>10.119199999999999</v>
+        <v>10.143890000000001</v>
       </c>
       <c r="D6" s="1">
-        <v>80.612489999999994</v>
+        <v>80.630089999999996</v>
       </c>
       <c r="E6" s="1">
-        <v>105.8317</v>
+        <v>105.871</v>
       </c>
       <c r="F6" s="1">
-        <v>4.9367479999999998E-2</v>
+        <v>4.9386029999999997E-2</v>
       </c>
       <c r="G6" s="1">
-        <v>0.9994767</v>
+        <v>0.99947750000000002</v>
       </c>
       <c r="H6" s="1">
-        <v>6.8773029999999999E-2</v>
+        <v>6.8739969999999997E-2</v>
       </c>
       <c r="I6" s="1">
-        <v>1.1616899999999999</v>
+        <v>1.1646399999999999</v>
       </c>
       <c r="J6" s="1">
-        <v>12.529400000000001</v>
+        <v>12.52176</v>
       </c>
       <c r="K6" s="1">
-        <v>0.25889659999999998</v>
+        <v>0.25987179999999999</v>
       </c>
       <c r="L6" s="1">
-        <v>1.224505</v>
+        <v>1.2263329999999999</v>
       </c>
       <c r="M6" s="1">
-        <v>0.18198259999999999</v>
+        <v>0.1825358</v>
       </c>
       <c r="N6" s="1">
-        <v>16.79899</v>
+        <v>16.797979999999999</v>
       </c>
       <c r="O6" s="1">
-        <v>999.41049999999996</v>
+        <v>999.41020000000003</v>
       </c>
       <c r="P6" s="1">
-        <v>46.887207119999999</v>
+        <v>46.887207719999999</v>
       </c>
       <c r="Q6" s="1">
-        <v>-91.050254019999997</v>
+        <v>-91.050270580000003</v>
       </c>
       <c r="R6" s="1"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
-        <v>45098.533275462964</v>
+        <v>45098.53328703704</v>
       </c>
       <c r="B7" s="1">
-        <v>6.2186240000000002</v>
+        <v>6.1674259999999999</v>
       </c>
       <c r="C7" s="1">
-        <v>10.143890000000001</v>
+        <v>10.44891</v>
       </c>
       <c r="D7" s="1">
-        <v>80.630089999999996</v>
+        <v>80.691689999999994</v>
       </c>
       <c r="E7" s="1">
-        <v>105.871</v>
+        <v>106.4443</v>
       </c>
       <c r="F7" s="1">
-        <v>4.9386029999999997E-2</v>
+        <v>4.9649819999999997E-2</v>
       </c>
       <c r="G7" s="1">
-        <v>0.99947750000000002</v>
+        <v>0.99950810000000001</v>
       </c>
       <c r="H7" s="1">
-        <v>6.8739969999999997E-2</v>
+        <v>6.9324179999999999E-2</v>
       </c>
       <c r="I7" s="1">
-        <v>1.1646399999999999</v>
+        <v>1.346857</v>
       </c>
       <c r="J7" s="1">
-        <v>12.52176</v>
+        <v>12.33512</v>
       </c>
       <c r="K7" s="1">
-        <v>0.25987179999999999</v>
+        <v>0.4206956</v>
       </c>
       <c r="L7" s="1">
-        <v>1.2263329999999999</v>
+        <v>1.588748</v>
       </c>
       <c r="M7" s="1">
-        <v>0.1825358</v>
+        <v>0.2957785</v>
       </c>
       <c r="N7" s="1">
-        <v>16.797979999999999</v>
+        <v>16.804839999999999</v>
       </c>
       <c r="O7" s="1">
-        <v>999.41020000000003</v>
+        <v>999.35709999999995</v>
       </c>
       <c r="P7" s="1">
         <v>46.887207719999999</v>
@@ -789,49 +840,49 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
-        <v>45098.53328703704</v>
+        <v>45098.53329861111</v>
       </c>
       <c r="B8" s="1">
-        <v>6.1674259999999999</v>
+        <v>6.1656500000000003</v>
       </c>
       <c r="C8" s="1">
-        <v>10.44891</v>
+        <v>10.472670000000001</v>
       </c>
       <c r="D8" s="1">
-        <v>80.691689999999994</v>
+        <v>80.705520000000007</v>
       </c>
       <c r="E8" s="1">
-        <v>106.4443</v>
+        <v>106.49209999999999</v>
       </c>
       <c r="F8" s="1">
-        <v>4.9649819999999997E-2</v>
+        <v>4.9672139999999997E-2</v>
       </c>
       <c r="G8" s="1">
-        <v>0.99950810000000001</v>
+        <v>0.99950989999999995</v>
       </c>
       <c r="H8" s="1">
-        <v>6.9324179999999999E-2</v>
+        <v>6.9362279999999998E-2</v>
       </c>
       <c r="I8" s="1">
-        <v>1.346857</v>
+        <v>1.3565119999999999</v>
       </c>
       <c r="J8" s="1">
-        <v>12.33512</v>
+        <v>12.322749999999999</v>
       </c>
       <c r="K8" s="1">
-        <v>0.4206956</v>
+        <v>0.42921290000000001</v>
       </c>
       <c r="L8" s="1">
-        <v>1.588748</v>
+        <v>1.6079129999999999</v>
       </c>
       <c r="M8" s="1">
-        <v>0.2957785</v>
+        <v>0.3017667</v>
       </c>
       <c r="N8" s="1">
-        <v>16.804839999999999</v>
+        <v>16.804569999999998</v>
       </c>
       <c r="O8" s="1">
-        <v>999.35709999999995</v>
+        <v>999.35410000000002</v>
       </c>
       <c r="P8" s="1">
         <v>46.887207719999999</v>
@@ -843,103 +894,103 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
-        <v>45098.53329861111</v>
+        <v>45098.533310185187</v>
       </c>
       <c r="B9" s="1">
-        <v>6.1656500000000003</v>
+        <v>6.163875</v>
       </c>
       <c r="C9" s="1">
-        <v>10.472670000000001</v>
+        <v>10.49644</v>
       </c>
       <c r="D9" s="1">
-        <v>80.705520000000007</v>
+        <v>80.719350000000006</v>
       </c>
       <c r="E9" s="1">
-        <v>106.49209999999999</v>
+        <v>106.54</v>
       </c>
       <c r="F9" s="1">
-        <v>4.9672139999999997E-2</v>
+        <v>4.9694460000000003E-2</v>
       </c>
       <c r="G9" s="1">
-        <v>0.99950989999999995</v>
+        <v>0.9995117</v>
       </c>
       <c r="H9" s="1">
-        <v>6.9362279999999998E-2</v>
+        <v>6.9400359999999994E-2</v>
       </c>
       <c r="I9" s="1">
-        <v>1.3565119999999999</v>
+        <v>1.3661669999999999</v>
       </c>
       <c r="J9" s="1">
-        <v>12.322749999999999</v>
+        <v>12.310370000000001</v>
       </c>
       <c r="K9" s="1">
-        <v>0.42921290000000001</v>
+        <v>0.43773030000000002</v>
       </c>
       <c r="L9" s="1">
-        <v>1.6079129999999999</v>
+        <v>1.627078</v>
       </c>
       <c r="M9" s="1">
-        <v>0.3017667</v>
+        <v>0.307755</v>
       </c>
       <c r="N9" s="1">
-        <v>16.804569999999998</v>
+        <v>16.804310000000001</v>
       </c>
       <c r="O9" s="1">
-        <v>999.35410000000002</v>
+        <v>999.35119999999995</v>
       </c>
       <c r="P9" s="1">
-        <v>46.887207719999999</v>
+        <v>46.887201060000002</v>
       </c>
       <c r="Q9" s="1">
-        <v>-91.050270580000003</v>
+        <v>-91.050251849999995</v>
       </c>
       <c r="R9" s="1"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
-        <v>45098.533310185187</v>
+        <v>45098.533321759256</v>
       </c>
       <c r="B10" s="1">
-        <v>6.163875</v>
+        <v>6.0639859999999999</v>
       </c>
       <c r="C10" s="1">
-        <v>10.49644</v>
+        <v>10.521319999999999</v>
       </c>
       <c r="D10" s="1">
-        <v>80.719350000000006</v>
+        <v>80.112210000000005</v>
       </c>
       <c r="E10" s="1">
-        <v>106.54</v>
+        <v>106.2217</v>
       </c>
       <c r="F10" s="1">
-        <v>4.9694460000000003E-2</v>
+        <v>4.9528389999999999E-2</v>
       </c>
       <c r="G10" s="1">
-        <v>0.9995117</v>
+        <v>0.99952439999999998</v>
       </c>
       <c r="H10" s="1">
-        <v>6.9400359999999994E-2</v>
+        <v>6.9059720000000005E-2</v>
       </c>
       <c r="I10" s="1">
-        <v>1.3661669999999999</v>
+        <v>1.099909</v>
       </c>
       <c r="J10" s="1">
-        <v>12.310370000000001</v>
+        <v>12.24147</v>
       </c>
       <c r="K10" s="1">
-        <v>0.43773030000000002</v>
+        <v>1.1596109999999999</v>
       </c>
       <c r="L10" s="1">
-        <v>1.627078</v>
+        <v>3.284456</v>
       </c>
       <c r="M10" s="1">
-        <v>0.307755</v>
+        <v>0.8152876</v>
       </c>
       <c r="N10" s="1">
-        <v>16.804310000000001</v>
+        <v>16.78905</v>
       </c>
       <c r="O10" s="1">
-        <v>999.35119999999995</v>
+        <v>999.36860000000001</v>
       </c>
       <c r="P10" s="1">
         <v>46.887201060000002</v>
@@ -951,49 +1002,49 @@
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
-        <v>45098.533321759256</v>
+        <v>45098.533333333333</v>
       </c>
       <c r="B11" s="1">
-        <v>6.0639859999999999</v>
+        <v>6.0578289999999999</v>
       </c>
       <c r="C11" s="1">
-        <v>10.521319999999999</v>
+        <v>10.529640000000001</v>
       </c>
       <c r="D11" s="1">
-        <v>80.112210000000005</v>
+        <v>80.082369999999997</v>
       </c>
       <c r="E11" s="1">
-        <v>106.2217</v>
+        <v>106.21810000000001</v>
       </c>
       <c r="F11" s="1">
-        <v>4.9528389999999999E-2</v>
+        <v>4.9525760000000002E-2</v>
       </c>
       <c r="G11" s="1">
-        <v>0.99952439999999998</v>
+        <v>0.99952569999999996</v>
       </c>
       <c r="H11" s="1">
-        <v>6.9059720000000005E-2</v>
+        <v>6.9053530000000002E-2</v>
       </c>
       <c r="I11" s="1">
-        <v>1.099909</v>
+        <v>1.0903069999999999</v>
       </c>
       <c r="J11" s="1">
-        <v>12.24147</v>
+        <v>12.233739999999999</v>
       </c>
       <c r="K11" s="1">
-        <v>1.1596109999999999</v>
+        <v>1.2002189999999999</v>
       </c>
       <c r="L11" s="1">
-        <v>3.284456</v>
+        <v>3.3775270000000002</v>
       </c>
       <c r="M11" s="1">
-        <v>0.8152876</v>
+        <v>0.84383770000000002</v>
       </c>
       <c r="N11" s="1">
-        <v>16.78905</v>
+        <v>16.788419999999999</v>
       </c>
       <c r="O11" s="1">
-        <v>999.36860000000001</v>
+        <v>999.36829999999998</v>
       </c>
       <c r="P11" s="1">
         <v>46.887201060000002</v>
@@ -1005,103 +1056,103 @@
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
-        <v>45098.533333333333</v>
+        <v>45098.53334490741</v>
       </c>
       <c r="B12" s="1">
-        <v>6.0578289999999999</v>
+        <v>6.0516719999999999</v>
       </c>
       <c r="C12" s="1">
-        <v>10.529640000000001</v>
+        <v>10.53795</v>
       </c>
       <c r="D12" s="1">
-        <v>80.082369999999997</v>
+        <v>80.052530000000004</v>
       </c>
       <c r="E12" s="1">
-        <v>106.21810000000001</v>
+        <v>106.2146</v>
       </c>
       <c r="F12" s="1">
-        <v>4.9525760000000002E-2</v>
+        <v>4.952314E-2</v>
       </c>
       <c r="G12" s="1">
-        <v>0.99952569999999996</v>
+        <v>0.99952700000000005</v>
       </c>
       <c r="H12" s="1">
-        <v>6.9053530000000002E-2</v>
+        <v>6.9047339999999999E-2</v>
       </c>
       <c r="I12" s="1">
-        <v>1.0903069999999999</v>
+        <v>1.0807040000000001</v>
       </c>
       <c r="J12" s="1">
-        <v>12.233739999999999</v>
+        <v>12.22602</v>
       </c>
       <c r="K12" s="1">
-        <v>1.2002189999999999</v>
+        <v>1.240826</v>
       </c>
       <c r="L12" s="1">
-        <v>3.3775270000000002</v>
+        <v>3.4705979999999998</v>
       </c>
       <c r="M12" s="1">
-        <v>0.84383770000000002</v>
+        <v>0.87238789999999999</v>
       </c>
       <c r="N12" s="1">
-        <v>16.788419999999999</v>
+        <v>16.787790000000001</v>
       </c>
       <c r="O12" s="1">
-        <v>999.36829999999998</v>
+        <v>999.36800000000005</v>
       </c>
       <c r="P12" s="1">
-        <v>46.887201060000002</v>
+        <v>46.88718678</v>
       </c>
       <c r="Q12" s="1">
-        <v>-91.050251849999995</v>
+        <v>-91.05025655</v>
       </c>
       <c r="R12" s="1"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
-        <v>45098.53334490741</v>
+        <v>45098.533356481479</v>
       </c>
       <c r="B13" s="1">
-        <v>6.0516719999999999</v>
+        <v>7.9907459999999997</v>
       </c>
       <c r="C13" s="1">
-        <v>10.53795</v>
+        <v>11.63795</v>
       </c>
       <c r="D13" s="1">
-        <v>80.052530000000004</v>
+        <v>79.17604</v>
       </c>
       <c r="E13" s="1">
-        <v>106.2146</v>
+        <v>105.6848</v>
       </c>
       <c r="F13" s="1">
-        <v>4.952314E-2</v>
+        <v>4.9250750000000003E-2</v>
       </c>
       <c r="G13" s="1">
-        <v>0.99952700000000005</v>
+        <v>0.99955340000000004</v>
       </c>
       <c r="H13" s="1">
-        <v>6.9047339999999999E-2</v>
+        <v>6.8699449999999995E-2</v>
       </c>
       <c r="I13" s="1">
-        <v>1.0807040000000001</v>
+        <v>0.93120130000000001</v>
       </c>
       <c r="J13" s="1">
-        <v>12.22602</v>
+        <v>11.880649999999999</v>
       </c>
       <c r="K13" s="1">
-        <v>1.240826</v>
+        <v>1.821172</v>
       </c>
       <c r="L13" s="1">
-        <v>3.4705979999999998</v>
+        <v>4.8135700000000003</v>
       </c>
       <c r="M13" s="1">
-        <v>0.87238789999999999</v>
+        <v>1.919554</v>
       </c>
       <c r="N13" s="1">
-        <v>16.787790000000001</v>
+        <v>16.693000000000001</v>
       </c>
       <c r="O13" s="1">
-        <v>999.36800000000005</v>
+        <v>999.40369999999996</v>
       </c>
       <c r="P13" s="1">
         <v>46.88718678</v>
@@ -1113,49 +1164,49 @@
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
-        <v>45098.533356481479</v>
+        <v>45098.533368055556</v>
       </c>
       <c r="B14" s="1">
-        <v>7.9907459999999997</v>
+        <v>8.0885379999999998</v>
       </c>
       <c r="C14" s="1">
-        <v>11.63795</v>
+        <v>11.69553</v>
       </c>
       <c r="D14" s="1">
-        <v>79.17604</v>
+        <v>79.117999999999995</v>
       </c>
       <c r="E14" s="1">
-        <v>105.6848</v>
+        <v>105.65130000000001</v>
       </c>
       <c r="F14" s="1">
-        <v>4.9250750000000003E-2</v>
+        <v>4.923346E-2</v>
       </c>
       <c r="G14" s="1">
-        <v>0.99955340000000004</v>
+        <v>0.99955510000000003</v>
       </c>
       <c r="H14" s="1">
-        <v>6.8699449999999995E-2</v>
+        <v>6.8674739999999998E-2</v>
       </c>
       <c r="I14" s="1">
-        <v>0.93120130000000001</v>
+        <v>0.91791020000000001</v>
       </c>
       <c r="J14" s="1">
-        <v>11.880649999999999</v>
+        <v>11.861179999999999</v>
       </c>
       <c r="K14" s="1">
-        <v>1.821172</v>
+        <v>1.866735</v>
       </c>
       <c r="L14" s="1">
-        <v>4.8135700000000003</v>
+        <v>4.9187159999999999</v>
       </c>
       <c r="M14" s="1">
-        <v>1.919554</v>
+        <v>1.9845379999999999</v>
       </c>
       <c r="N14" s="1">
-        <v>16.693000000000001</v>
+        <v>16.68779</v>
       </c>
       <c r="O14" s="1">
-        <v>999.40369999999996</v>
+        <v>999.40589999999997</v>
       </c>
       <c r="P14" s="1">
         <v>46.88718678</v>
@@ -1167,49 +1218,49 @@
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
-        <v>45098.533368055556</v>
+        <v>45098.533379629633</v>
       </c>
       <c r="B15" s="1">
-        <v>8.0885379999999998</v>
+        <v>8.1863309999999991</v>
       </c>
       <c r="C15" s="1">
-        <v>11.69553</v>
+        <v>11.753119999999999</v>
       </c>
       <c r="D15" s="1">
-        <v>79.117999999999995</v>
+        <v>79.059939999999997</v>
       </c>
       <c r="E15" s="1">
-        <v>105.65130000000001</v>
+        <v>105.61790000000001</v>
       </c>
       <c r="F15" s="1">
-        <v>4.923346E-2</v>
+        <v>4.9216169999999997E-2</v>
       </c>
       <c r="G15" s="1">
-        <v>0.99955510000000003</v>
+        <v>0.99955680000000002</v>
       </c>
       <c r="H15" s="1">
-        <v>6.8674739999999998E-2</v>
+        <v>6.8650030000000001E-2</v>
       </c>
       <c r="I15" s="1">
-        <v>0.91791020000000001</v>
+        <v>0.90461910000000001</v>
       </c>
       <c r="J15" s="1">
-        <v>11.861179999999999</v>
+        <v>11.84172</v>
       </c>
       <c r="K15" s="1">
-        <v>1.866735</v>
+        <v>1.9122980000000001</v>
       </c>
       <c r="L15" s="1">
-        <v>4.9187159999999999</v>
+        <v>5.0238620000000003</v>
       </c>
       <c r="M15" s="1">
-        <v>1.9845379999999999</v>
+        <v>2.0495220000000001</v>
       </c>
       <c r="N15" s="1">
-        <v>16.68779</v>
+        <v>16.682569999999998</v>
       </c>
       <c r="O15" s="1">
-        <v>999.40589999999997</v>
+        <v>999.40809999999999</v>
       </c>
       <c r="P15" s="1">
         <v>46.88718678</v>
@@ -1221,49 +1272,49 @@
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
-        <v>45098.533379629633</v>
+        <v>45098.533391203702</v>
       </c>
       <c r="B16" s="1">
-        <v>8.1863309999999991</v>
+        <v>8.2403359999999992</v>
       </c>
       <c r="C16" s="1">
-        <v>11.753119999999999</v>
+        <v>11.945</v>
       </c>
       <c r="D16" s="1">
-        <v>79.059939999999997</v>
+        <v>77.701520000000002</v>
       </c>
       <c r="E16" s="1">
-        <v>105.61790000000001</v>
+        <v>104.86879999999999</v>
       </c>
       <c r="F16" s="1">
-        <v>4.9216169999999997E-2</v>
+        <v>4.8825140000000003E-2</v>
       </c>
       <c r="G16" s="1">
-        <v>0.99955680000000002</v>
+        <v>0.99960009999999999</v>
       </c>
       <c r="H16" s="1">
-        <v>6.8650030000000001E-2</v>
+        <v>6.8164710000000003E-2</v>
       </c>
       <c r="I16" s="1">
-        <v>0.90461910000000001</v>
+        <v>1.023647</v>
       </c>
       <c r="J16" s="1">
-        <v>11.84172</v>
+        <v>11.624919999999999</v>
       </c>
       <c r="K16" s="1">
-        <v>1.9122980000000001</v>
+        <v>3.702855</v>
       </c>
       <c r="L16" s="1">
-        <v>5.0238620000000003</v>
+        <v>9.1644570000000005</v>
       </c>
       <c r="M16" s="1">
-        <v>2.0495220000000001</v>
+        <v>2.6851820000000002</v>
       </c>
       <c r="N16" s="1">
-        <v>16.682569999999998</v>
+        <v>16.790330000000001</v>
       </c>
       <c r="O16" s="1">
-        <v>999.40809999999999</v>
+        <v>999.42550000000006</v>
       </c>
       <c r="P16" s="1">
         <v>46.88718678</v>
@@ -1275,49 +1326,49 @@
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
-        <v>45098.533391203702</v>
+        <v>45098.533402777779</v>
       </c>
       <c r="B17" s="1">
-        <v>8.2403359999999992</v>
+        <v>8.2845359999999992</v>
       </c>
       <c r="C17" s="1">
-        <v>11.945</v>
+        <v>11.978529999999999</v>
       </c>
       <c r="D17" s="1">
-        <v>77.701520000000002</v>
+        <v>77.612629999999996</v>
       </c>
       <c r="E17" s="1">
-        <v>104.86879999999999</v>
+        <v>104.819</v>
       </c>
       <c r="F17" s="1">
-        <v>4.8825140000000003E-2</v>
+        <v>4.8799210000000003E-2</v>
       </c>
       <c r="G17" s="1">
-        <v>0.99960009999999999</v>
+        <v>0.99960289999999996</v>
       </c>
       <c r="H17" s="1">
-        <v>6.8164710000000003E-2</v>
+        <v>6.8132330000000005E-2</v>
       </c>
       <c r="I17" s="1">
-        <v>1.023647</v>
+        <v>1.026535</v>
       </c>
       <c r="J17" s="1">
-        <v>11.624919999999999</v>
+        <v>11.60628</v>
       </c>
       <c r="K17" s="1">
-        <v>3.702855</v>
+        <v>3.8077839999999998</v>
       </c>
       <c r="L17" s="1">
-        <v>9.1644570000000005</v>
+        <v>9.407114</v>
       </c>
       <c r="M17" s="1">
-        <v>2.6851820000000002</v>
+        <v>2.740542</v>
       </c>
       <c r="N17" s="1">
-        <v>16.790330000000001</v>
+        <v>16.793849999999999</v>
       </c>
       <c r="O17" s="1">
-        <v>999.42550000000006</v>
+        <v>999.42719999999997</v>
       </c>
       <c r="P17" s="1">
         <v>46.88718678</v>
@@ -1329,103 +1380,103 @@
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
-        <v>45098.533402777779</v>
+        <v>45098.533414351848</v>
       </c>
       <c r="B18" s="1">
-        <v>8.2845359999999992</v>
+        <v>8.328735</v>
       </c>
       <c r="C18" s="1">
-        <v>11.978529999999999</v>
+        <v>12.01205</v>
       </c>
       <c r="D18" s="1">
-        <v>77.612629999999996</v>
+        <v>77.52373</v>
       </c>
       <c r="E18" s="1">
-        <v>104.819</v>
+        <v>104.76909999999999</v>
       </c>
       <c r="F18" s="1">
-        <v>4.8799210000000003E-2</v>
+        <v>4.8773280000000002E-2</v>
       </c>
       <c r="G18" s="1">
-        <v>0.99960289999999996</v>
+        <v>0.99960570000000004</v>
       </c>
       <c r="H18" s="1">
-        <v>6.8132330000000005E-2</v>
+        <v>6.8099950000000006E-2</v>
       </c>
       <c r="I18" s="1">
-        <v>1.026535</v>
+        <v>1.029423</v>
       </c>
       <c r="J18" s="1">
-        <v>11.60628</v>
+        <v>11.58764</v>
       </c>
       <c r="K18" s="1">
-        <v>3.8077839999999998</v>
+        <v>3.9127130000000001</v>
       </c>
       <c r="L18" s="1">
-        <v>9.407114</v>
+        <v>9.6497700000000002</v>
       </c>
       <c r="M18" s="1">
-        <v>2.740542</v>
+        <v>2.795903</v>
       </c>
       <c r="N18" s="1">
-        <v>16.793849999999999</v>
+        <v>16.797370000000001</v>
       </c>
       <c r="O18" s="1">
-        <v>999.42719999999997</v>
+        <v>999.42880000000002</v>
       </c>
       <c r="P18" s="1">
-        <v>46.88718678</v>
+        <v>46.887177370000003</v>
       </c>
       <c r="Q18" s="1">
-        <v>-91.05025655</v>
+        <v>-91.050247909999996</v>
       </c>
       <c r="R18" s="1"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
-        <v>45098.533414351848</v>
+        <v>45098.533425925925</v>
       </c>
       <c r="B19" s="1">
-        <v>8.328735</v>
+        <v>8.5752989999999993</v>
       </c>
       <c r="C19" s="1">
-        <v>12.01205</v>
+        <v>12.19089</v>
       </c>
       <c r="D19" s="1">
-        <v>77.52373</v>
+        <v>76.596029999999999</v>
       </c>
       <c r="E19" s="1">
-        <v>104.76909999999999</v>
+        <v>104.16249999999999</v>
       </c>
       <c r="F19" s="1">
-        <v>4.8773280000000002E-2</v>
+        <v>4.8462159999999997E-2</v>
       </c>
       <c r="G19" s="1">
-        <v>0.99960570000000004</v>
+        <v>0.99963060000000004</v>
       </c>
       <c r="H19" s="1">
-        <v>6.8099950000000006E-2</v>
+        <v>6.7705639999999997E-2</v>
       </c>
       <c r="I19" s="1">
-        <v>1.029423</v>
+        <v>1.0290969999999999</v>
       </c>
       <c r="J19" s="1">
-        <v>11.58764</v>
+        <v>11.16779</v>
       </c>
       <c r="K19" s="1">
-        <v>3.9127130000000001</v>
+        <v>4.8023559999999996</v>
       </c>
       <c r="L19" s="1">
-        <v>9.6497700000000002</v>
+        <v>11.70309</v>
       </c>
       <c r="M19" s="1">
-        <v>2.795903</v>
+        <v>3.4024610000000002</v>
       </c>
       <c r="N19" s="1">
-        <v>16.797370000000001</v>
+        <v>16.83118</v>
       </c>
       <c r="O19" s="1">
-        <v>999.42880000000002</v>
+        <v>999.39490000000001</v>
       </c>
       <c r="P19" s="1">
         <v>46.887177370000003</v>
@@ -1437,49 +1488,49 @@
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
-        <v>45098.533425925925</v>
+        <v>45098.533437500002</v>
       </c>
       <c r="B20" s="1">
-        <v>8.5752989999999993</v>
+        <v>8.5894929999999992</v>
       </c>
       <c r="C20" s="1">
-        <v>12.19089</v>
+        <v>12.204370000000001</v>
       </c>
       <c r="D20" s="1">
-        <v>76.596029999999999</v>
+        <v>76.518950000000004</v>
       </c>
       <c r="E20" s="1">
-        <v>104.16249999999999</v>
+        <v>104.11499999999999</v>
       </c>
       <c r="F20" s="1">
-        <v>4.8462159999999997E-2</v>
+        <v>4.8437670000000002E-2</v>
       </c>
       <c r="G20" s="1">
-        <v>0.99963060000000004</v>
+        <v>0.99963279999999999</v>
       </c>
       <c r="H20" s="1">
-        <v>6.7705639999999997E-2</v>
+        <v>6.7674789999999999E-2</v>
       </c>
       <c r="I20" s="1">
-        <v>1.0290969999999999</v>
+        <v>1.0314859999999999</v>
       </c>
       <c r="J20" s="1">
-        <v>11.16779</v>
+        <v>11.14128</v>
       </c>
       <c r="K20" s="1">
-        <v>4.8023559999999996</v>
+        <v>4.8864749999999999</v>
       </c>
       <c r="L20" s="1">
-        <v>11.70309</v>
+        <v>11.897399999999999</v>
       </c>
       <c r="M20" s="1">
-        <v>3.4024610000000002</v>
+        <v>3.4476589999999998</v>
       </c>
       <c r="N20" s="1">
-        <v>16.83118</v>
+        <v>16.835190000000001</v>
       </c>
       <c r="O20" s="1">
-        <v>999.39490000000001</v>
+        <v>999.39350000000002</v>
       </c>
       <c r="P20" s="1">
         <v>46.887177370000003</v>
@@ -1491,49 +1542,49 @@
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
-        <v>45098.533437500002</v>
+        <v>45098.533449074072</v>
       </c>
       <c r="B21" s="1">
-        <v>8.5894929999999992</v>
+        <v>8.6036859999999997</v>
       </c>
       <c r="C21" s="1">
-        <v>12.204370000000001</v>
+        <v>12.21785</v>
       </c>
       <c r="D21" s="1">
-        <v>76.518950000000004</v>
+        <v>76.441879999999998</v>
       </c>
       <c r="E21" s="1">
-        <v>104.11499999999999</v>
+        <v>104.0676</v>
       </c>
       <c r="F21" s="1">
-        <v>4.8437670000000002E-2</v>
+        <v>4.841318E-2</v>
       </c>
       <c r="G21" s="1">
-        <v>0.99963279999999999</v>
+        <v>0.99963500000000005</v>
       </c>
       <c r="H21" s="1">
-        <v>6.7674789999999999E-2</v>
+        <v>6.7643930000000005E-2</v>
       </c>
       <c r="I21" s="1">
-        <v>1.0314859999999999</v>
+        <v>1.0338750000000001</v>
       </c>
       <c r="J21" s="1">
-        <v>11.14128</v>
+        <v>11.11477</v>
       </c>
       <c r="K21" s="1">
-        <v>4.8864749999999999</v>
+        <v>4.970593</v>
       </c>
       <c r="L21" s="1">
-        <v>11.897399999999999</v>
+        <v>12.09172</v>
       </c>
       <c r="M21" s="1">
-        <v>3.4476589999999998</v>
+        <v>3.492858</v>
       </c>
       <c r="N21" s="1">
-        <v>16.835190000000001</v>
+        <v>16.839189999999999</v>
       </c>
       <c r="O21" s="1">
-        <v>999.39350000000002</v>
+        <v>999.39210000000003</v>
       </c>
       <c r="P21" s="1">
         <v>46.887177370000003</v>
@@ -1545,49 +1596,49 @@
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
-        <v>45098.533449074072</v>
+        <v>45098.533460648148</v>
       </c>
       <c r="B22" s="1">
-        <v>8.6036859999999997</v>
+        <v>8.4033040000000003</v>
       </c>
       <c r="C22" s="1">
-        <v>12.21785</v>
+        <v>12.915469999999999</v>
       </c>
       <c r="D22" s="1">
-        <v>76.441879999999998</v>
+        <v>74.129289999999997</v>
       </c>
       <c r="E22" s="1">
-        <v>104.0676</v>
+        <v>101.6292</v>
       </c>
       <c r="F22" s="1">
-        <v>4.841318E-2</v>
+        <v>4.7218349999999999E-2</v>
       </c>
       <c r="G22" s="1">
-        <v>0.99963500000000005</v>
+        <v>0.99971520000000003</v>
       </c>
       <c r="H22" s="1">
-        <v>6.7643930000000005E-2</v>
+        <v>6.4274929999999994E-2</v>
       </c>
       <c r="I22" s="1">
-        <v>1.0338750000000001</v>
+        <v>1.158628</v>
       </c>
       <c r="J22" s="1">
-        <v>11.11477</v>
+        <v>10.83963</v>
       </c>
       <c r="K22" s="1">
-        <v>4.970593</v>
+        <v>7.1816709999999997</v>
       </c>
       <c r="L22" s="1">
-        <v>12.09172</v>
+        <v>17.1907</v>
       </c>
       <c r="M22" s="1">
-        <v>3.492858</v>
+        <v>5.0492179999999998</v>
       </c>
       <c r="N22" s="1">
-        <v>16.839189999999999</v>
+        <v>16.809290000000001</v>
       </c>
       <c r="O22" s="1">
-        <v>999.39210000000003</v>
+        <v>999.40800000000002</v>
       </c>
       <c r="P22" s="1">
         <v>46.887177370000003</v>
@@ -1599,49 +1650,49 @@
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
-        <v>45098.533460648148</v>
+        <v>45098.533472222225</v>
       </c>
       <c r="B23" s="1">
-        <v>8.4033040000000003</v>
+        <v>8.3983439999999998</v>
       </c>
       <c r="C23" s="1">
-        <v>12.915469999999999</v>
+        <v>12.95581</v>
       </c>
       <c r="D23" s="1">
-        <v>74.129289999999997</v>
+        <v>73.989189999999994</v>
       </c>
       <c r="E23" s="1">
-        <v>101.6292</v>
+        <v>101.4892</v>
       </c>
       <c r="F23" s="1">
-        <v>4.7218349999999999E-2</v>
+        <v>4.7149440000000001E-2</v>
       </c>
       <c r="G23" s="1">
-        <v>0.99971520000000003</v>
+        <v>0.99971989999999999</v>
       </c>
       <c r="H23" s="1">
-        <v>6.4274929999999994E-2</v>
+        <v>6.4090709999999995E-2</v>
       </c>
       <c r="I23" s="1">
-        <v>1.158628</v>
+        <v>1.1650780000000001</v>
       </c>
       <c r="J23" s="1">
-        <v>10.83963</v>
+        <v>10.8164</v>
       </c>
       <c r="K23" s="1">
-        <v>7.1816709999999997</v>
+        <v>7.3154789999999998</v>
       </c>
       <c r="L23" s="1">
-        <v>17.1907</v>
+        <v>17.499310000000001</v>
       </c>
       <c r="M23" s="1">
-        <v>5.0492179999999998</v>
+        <v>5.143294</v>
       </c>
       <c r="N23" s="1">
-        <v>16.809290000000001</v>
+        <v>16.808399999999999</v>
       </c>
       <c r="O23" s="1">
-        <v>999.40800000000002</v>
+        <v>999.40809999999999</v>
       </c>
       <c r="P23" s="1">
         <v>46.887177370000003</v>
@@ -1653,49 +1704,49 @@
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
-        <v>45098.533472222225</v>
+        <v>45098.533483796295</v>
       </c>
       <c r="B24" s="1">
-        <v>8.3983439999999998</v>
+        <v>8.3933850000000003</v>
       </c>
       <c r="C24" s="1">
-        <v>12.95581</v>
+        <v>12.99615</v>
       </c>
       <c r="D24" s="1">
-        <v>73.989189999999994</v>
+        <v>73.849080000000001</v>
       </c>
       <c r="E24" s="1">
-        <v>101.4892</v>
+        <v>101.3492</v>
       </c>
       <c r="F24" s="1">
-        <v>4.7149440000000001E-2</v>
+        <v>4.7080539999999997E-2</v>
       </c>
       <c r="G24" s="1">
-        <v>0.99971989999999999</v>
+        <v>0.99972459999999996</v>
       </c>
       <c r="H24" s="1">
-        <v>6.4090709999999995E-2</v>
+        <v>6.3906489999999996E-2</v>
       </c>
       <c r="I24" s="1">
-        <v>1.1650780000000001</v>
+        <v>1.171527</v>
       </c>
       <c r="J24" s="1">
-        <v>10.8164</v>
+        <v>10.79318</v>
       </c>
       <c r="K24" s="1">
-        <v>7.3154789999999998</v>
+        <v>7.449287</v>
       </c>
       <c r="L24" s="1">
-        <v>17.499310000000001</v>
+        <v>17.807919999999999</v>
       </c>
       <c r="M24" s="1">
-        <v>5.143294</v>
+        <v>5.2373700000000003</v>
       </c>
       <c r="N24" s="1">
-        <v>16.808399999999999</v>
+        <v>16.807500000000001</v>
       </c>
       <c r="O24" s="1">
-        <v>999.40809999999999</v>
+        <v>999.40819999999997</v>
       </c>
       <c r="P24" s="1">
         <v>46.887177370000003</v>
@@ -1707,103 +1758,103 @@
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
-        <v>45098.533483796295</v>
+        <v>45098.533495370371</v>
       </c>
       <c r="B25" s="1">
-        <v>8.3933850000000003</v>
+        <v>8.3884249999999998</v>
       </c>
       <c r="C25" s="1">
-        <v>12.99615</v>
+        <v>13.036490000000001</v>
       </c>
       <c r="D25" s="1">
-        <v>73.849080000000001</v>
+        <v>73.708979999999997</v>
       </c>
       <c r="E25" s="1">
-        <v>101.3492</v>
+        <v>101.20910000000001</v>
       </c>
       <c r="F25" s="1">
-        <v>4.7080539999999997E-2</v>
+        <v>4.701164E-2</v>
       </c>
       <c r="G25" s="1">
-        <v>0.99972459999999996</v>
+        <v>0.99972930000000004</v>
       </c>
       <c r="H25" s="1">
-        <v>6.3906489999999996E-2</v>
+        <v>6.3722280000000006E-2</v>
       </c>
       <c r="I25" s="1">
-        <v>1.171527</v>
+        <v>1.1779770000000001</v>
       </c>
       <c r="J25" s="1">
-        <v>10.79318</v>
+        <v>10.76995</v>
       </c>
       <c r="K25" s="1">
-        <v>7.449287</v>
+        <v>7.5830950000000001</v>
       </c>
       <c r="L25" s="1">
-        <v>17.807919999999999</v>
+        <v>18.116530000000001</v>
       </c>
       <c r="M25" s="1">
-        <v>5.2373700000000003</v>
+        <v>5.3314469999999998</v>
       </c>
       <c r="N25" s="1">
-        <v>16.807500000000001</v>
+        <v>16.8066</v>
       </c>
       <c r="O25" s="1">
-        <v>999.40819999999997</v>
+        <v>999.40830000000005</v>
       </c>
       <c r="P25" s="1">
-        <v>46.887177370000003</v>
+        <v>46.887170220000002</v>
       </c>
       <c r="Q25" s="1">
-        <v>-91.050247909999996</v>
+        <v>-91.050230069999998</v>
       </c>
       <c r="R25" s="1"/>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
-        <v>45098.533495370371</v>
+        <v>45098.533506944441</v>
       </c>
       <c r="B26" s="1">
-        <v>8.3884249999999998</v>
+        <v>8.785266</v>
       </c>
       <c r="C26" s="1">
-        <v>13.036490000000001</v>
+        <v>13.41319</v>
       </c>
       <c r="D26" s="1">
-        <v>73.708979999999997</v>
+        <v>68.381799999999998</v>
       </c>
       <c r="E26" s="1">
-        <v>101.20910000000001</v>
+        <v>97.711560000000006</v>
       </c>
       <c r="F26" s="1">
-        <v>4.701164E-2</v>
+        <v>4.5195829999999999E-2</v>
       </c>
       <c r="G26" s="1">
-        <v>0.99972930000000004</v>
+        <v>0.99980190000000002</v>
       </c>
       <c r="H26" s="1">
-        <v>6.3722280000000006E-2</v>
+        <v>6.331328E-2</v>
       </c>
       <c r="I26" s="1">
-        <v>1.1779770000000001</v>
+        <v>1.089054</v>
       </c>
       <c r="J26" s="1">
-        <v>10.76995</v>
+        <v>10.163309999999999</v>
       </c>
       <c r="K26" s="1">
-        <v>7.5830950000000001</v>
+        <v>8.7340389999999992</v>
       </c>
       <c r="L26" s="1">
-        <v>18.116530000000001</v>
+        <v>20.774750000000001</v>
       </c>
       <c r="M26" s="1">
-        <v>5.3314469999999998</v>
+        <v>6.1406409999999996</v>
       </c>
       <c r="N26" s="1">
-        <v>16.8066</v>
+        <v>16.79786</v>
       </c>
       <c r="O26" s="1">
-        <v>999.40830000000005</v>
+        <v>999.40920000000006</v>
       </c>
       <c r="P26" s="1">
         <v>46.887170220000002</v>
@@ -1815,103 +1866,103 @@
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
-        <v>45098.533506944441</v>
+        <v>45098.533518518518</v>
       </c>
       <c r="B27" s="1">
-        <v>8.785266</v>
+        <v>8.8010420000000007</v>
       </c>
       <c r="C27" s="1">
-        <v>13.41319</v>
+        <v>13.447850000000001</v>
       </c>
       <c r="D27" s="1">
-        <v>68.381799999999998</v>
+        <v>68.060360000000003</v>
       </c>
       <c r="E27" s="1">
-        <v>97.711560000000006</v>
+        <v>97.480099999999993</v>
       </c>
       <c r="F27" s="1">
-        <v>4.5195829999999999E-2</v>
+        <v>4.5077249999999999E-2</v>
       </c>
       <c r="G27" s="1">
-        <v>0.99980190000000002</v>
+        <v>0.99980740000000001</v>
       </c>
       <c r="H27" s="1">
-        <v>6.331328E-2</v>
+        <v>6.3217510000000005E-2</v>
       </c>
       <c r="I27" s="1">
-        <v>1.089054</v>
+        <v>1.0873330000000001</v>
       </c>
       <c r="J27" s="1">
-        <v>10.163309999999999</v>
+        <v>10.12626</v>
       </c>
       <c r="K27" s="1">
-        <v>8.7340389999999992</v>
+        <v>8.8419810000000005</v>
       </c>
       <c r="L27" s="1">
-        <v>20.774750000000001</v>
+        <v>21.023879999999998</v>
       </c>
       <c r="M27" s="1">
-        <v>6.1406409999999996</v>
+        <v>6.2165319999999999</v>
       </c>
       <c r="N27" s="1">
-        <v>16.79786</v>
+        <v>16.796779999999998</v>
       </c>
       <c r="O27" s="1">
-        <v>999.40920000000006</v>
+        <v>999.40949999999998</v>
       </c>
       <c r="P27" s="1">
-        <v>46.887170220000002</v>
+        <v>46.887168860000003</v>
       </c>
       <c r="Q27" s="1">
-        <v>-91.050230069999998</v>
+        <v>-91.050215499999993</v>
       </c>
       <c r="R27" s="1"/>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
-        <v>45098.533518518518</v>
+        <v>45098.533530092594</v>
       </c>
       <c r="B28" s="1">
-        <v>8.8010420000000007</v>
+        <v>8.8168170000000003</v>
       </c>
       <c r="C28" s="1">
-        <v>13.447850000000001</v>
+        <v>13.482519999999999</v>
       </c>
       <c r="D28" s="1">
-        <v>68.060360000000003</v>
+        <v>67.738919999999993</v>
       </c>
       <c r="E28" s="1">
-        <v>97.480099999999993</v>
+        <v>97.248630000000006</v>
       </c>
       <c r="F28" s="1">
-        <v>4.5077249999999999E-2</v>
+        <v>4.4958659999999998E-2</v>
       </c>
       <c r="G28" s="1">
-        <v>0.99980740000000001</v>
+        <v>0.9998129</v>
       </c>
       <c r="H28" s="1">
-        <v>6.3217510000000005E-2</v>
+        <v>6.3121739999999996E-2</v>
       </c>
       <c r="I28" s="1">
-        <v>1.0873330000000001</v>
+        <v>1.0856110000000001</v>
       </c>
       <c r="J28" s="1">
-        <v>10.12626</v>
+        <v>10.08921</v>
       </c>
       <c r="K28" s="1">
-        <v>8.8419810000000005</v>
+        <v>8.9499239999999993</v>
       </c>
       <c r="L28" s="1">
-        <v>21.023879999999998</v>
+        <v>21.273009999999999</v>
       </c>
       <c r="M28" s="1">
-        <v>6.2165319999999999</v>
+        <v>6.2924220000000002</v>
       </c>
       <c r="N28" s="1">
-        <v>16.796779999999998</v>
+        <v>16.7957</v>
       </c>
       <c r="O28" s="1">
-        <v>999.40949999999998</v>
+        <v>999.40989999999999</v>
       </c>
       <c r="P28" s="1">
         <v>46.887168860000003</v>
@@ -1923,49 +1974,49 @@
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
-        <v>45098.533530092594</v>
+        <v>45098.533541666664</v>
       </c>
       <c r="B29" s="1">
-        <v>8.8168170000000003</v>
+        <v>9.3275900000000007</v>
       </c>
       <c r="C29" s="1">
-        <v>13.482519999999999</v>
+        <v>13.39044</v>
       </c>
       <c r="D29" s="1">
-        <v>67.738919999999993</v>
+        <v>67.347560000000001</v>
       </c>
       <c r="E29" s="1">
-        <v>97.248630000000006</v>
+        <v>98.086920000000006</v>
       </c>
       <c r="F29" s="1">
-        <v>4.4958659999999998E-2</v>
+        <v>4.5305749999999999E-2</v>
       </c>
       <c r="G29" s="1">
-        <v>0.9998129</v>
+        <v>0.99984919999999999</v>
       </c>
       <c r="H29" s="1">
-        <v>6.3121739999999996E-2</v>
+        <v>6.3705650000000003E-2</v>
       </c>
       <c r="I29" s="1">
-        <v>1.0856110000000001</v>
+        <v>1.1631480000000001</v>
       </c>
       <c r="J29" s="1">
-        <v>10.08921</v>
+        <v>8.6902000000000008</v>
       </c>
       <c r="K29" s="1">
-        <v>8.9499239999999993</v>
+        <v>10.01445</v>
       </c>
       <c r="L29" s="1">
-        <v>21.273009999999999</v>
+        <v>25.22326</v>
       </c>
       <c r="M29" s="1">
-        <v>6.2924220000000002</v>
+        <v>7.4980510000000002</v>
       </c>
       <c r="N29" s="1">
-        <v>16.7957</v>
+        <v>16.804110000000001</v>
       </c>
       <c r="O29" s="1">
-        <v>999.40989999999999</v>
+        <v>999.37450000000001</v>
       </c>
       <c r="P29" s="1">
         <v>46.887168860000003</v>
@@ -1977,49 +2028,49 @@
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
-        <v>45098.533541666664</v>
+        <v>45098.533553240741</v>
       </c>
       <c r="B30" s="1">
-        <v>9.3275900000000007</v>
+        <v>9.3620750000000008</v>
       </c>
       <c r="C30" s="1">
-        <v>13.39044</v>
+        <v>13.39451</v>
       </c>
       <c r="D30" s="1">
-        <v>67.347560000000001</v>
+        <v>67.210830000000001</v>
       </c>
       <c r="E30" s="1">
-        <v>98.086920000000006</v>
+        <v>98.052149999999997</v>
       </c>
       <c r="F30" s="1">
-        <v>4.5305749999999999E-2</v>
+        <v>4.5283280000000002E-2</v>
       </c>
       <c r="G30" s="1">
-        <v>0.99984919999999999</v>
+        <v>0.99985270000000004</v>
       </c>
       <c r="H30" s="1">
-        <v>6.3705650000000003E-2</v>
+        <v>6.3723589999999997E-2</v>
       </c>
       <c r="I30" s="1">
-        <v>1.1631480000000001</v>
+        <v>1.165289</v>
       </c>
       <c r="J30" s="1">
-        <v>8.6902000000000008</v>
+        <v>8.6055089999999996</v>
       </c>
       <c r="K30" s="1">
-        <v>10.01445</v>
+        <v>10.09563</v>
       </c>
       <c r="L30" s="1">
-        <v>25.22326</v>
+        <v>25.486699999999999</v>
       </c>
       <c r="M30" s="1">
-        <v>7.4980510000000002</v>
+        <v>7.5784050000000001</v>
       </c>
       <c r="N30" s="1">
-        <v>16.804110000000001</v>
+        <v>16.80434</v>
       </c>
       <c r="O30" s="1">
-        <v>999.37450000000001</v>
+        <v>999.37270000000001</v>
       </c>
       <c r="P30" s="1">
         <v>46.887168860000003</v>
@@ -2031,49 +2082,49 @@
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
-        <v>45098.533553240741</v>
+        <v>45098.533564814818</v>
       </c>
       <c r="B31" s="1">
-        <v>9.3620750000000008</v>
+        <v>9.3965610000000002</v>
       </c>
       <c r="C31" s="1">
-        <v>13.39451</v>
+        <v>13.398580000000001</v>
       </c>
       <c r="D31" s="1">
-        <v>67.210830000000001</v>
+        <v>67.074089999999998</v>
       </c>
       <c r="E31" s="1">
-        <v>98.052149999999997</v>
+        <v>98.017359999999996</v>
       </c>
       <c r="F31" s="1">
-        <v>4.5283280000000002E-2</v>
+        <v>4.5260790000000002E-2</v>
       </c>
       <c r="G31" s="1">
-        <v>0.99985270000000004</v>
+        <v>0.99985619999999997</v>
       </c>
       <c r="H31" s="1">
-        <v>6.3723589999999997E-2</v>
+        <v>6.3741530000000005E-2</v>
       </c>
       <c r="I31" s="1">
-        <v>1.165289</v>
+        <v>1.1674290000000001</v>
       </c>
       <c r="J31" s="1">
-        <v>8.6055089999999996</v>
+        <v>8.5208180000000002</v>
       </c>
       <c r="K31" s="1">
-        <v>10.09563</v>
+        <v>10.17681</v>
       </c>
       <c r="L31" s="1">
-        <v>25.486699999999999</v>
+        <v>25.750129999999999</v>
       </c>
       <c r="M31" s="1">
-        <v>7.5784050000000001</v>
+        <v>7.6587589999999999</v>
       </c>
       <c r="N31" s="1">
-        <v>16.80434</v>
+        <v>16.804569999999998</v>
       </c>
       <c r="O31" s="1">
-        <v>999.37270000000001</v>
+        <v>999.37099999999998</v>
       </c>
       <c r="P31" s="1">
         <v>46.887168860000003</v>
@@ -2085,49 +2136,49 @@
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
-        <v>45098.533564814818</v>
+        <v>45098.533576388887</v>
       </c>
       <c r="B32" s="1">
-        <v>9.3965610000000002</v>
+        <v>9.1937080000000009</v>
       </c>
       <c r="C32" s="1">
-        <v>13.398580000000001</v>
+        <v>13.474299999999999</v>
       </c>
       <c r="D32" s="1">
-        <v>67.074089999999998</v>
+        <v>66.489649999999997</v>
       </c>
       <c r="E32" s="1">
-        <v>98.017359999999996</v>
+        <v>98.43562</v>
       </c>
       <c r="F32" s="1">
-        <v>4.5260790000000002E-2</v>
+        <v>4.5407879999999998E-2</v>
       </c>
       <c r="G32" s="1">
-        <v>0.99985619999999997</v>
+        <v>0.99988600000000005</v>
       </c>
       <c r="H32" s="1">
-        <v>6.3741530000000005E-2</v>
+        <v>6.3983150000000003E-2</v>
       </c>
       <c r="I32" s="1">
-        <v>1.1674290000000001</v>
+        <v>1.3688689999999999</v>
       </c>
       <c r="J32" s="1">
-        <v>8.5208180000000002</v>
+        <v>8.2208380000000005</v>
       </c>
       <c r="K32" s="1">
-        <v>10.17681</v>
+        <v>11.849769999999999</v>
       </c>
       <c r="L32" s="1">
-        <v>25.750129999999999</v>
+        <v>28.13618</v>
       </c>
       <c r="M32" s="1">
-        <v>7.6587589999999999</v>
+        <v>8.3848730000000007</v>
       </c>
       <c r="N32" s="1">
-        <v>16.804569999999998</v>
+        <v>16.71773</v>
       </c>
       <c r="O32" s="1">
-        <v>999.37099999999998</v>
+        <v>999.40549999999996</v>
       </c>
       <c r="P32" s="1">
         <v>46.887168860000003</v>
@@ -2139,49 +2190,49 @@
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
-        <v>45098.533576388887</v>
+        <v>45098.533587962964</v>
       </c>
       <c r="B33" s="1">
-        <v>9.1937080000000009</v>
+        <v>9.194502</v>
       </c>
       <c r="C33" s="1">
-        <v>13.474299999999999</v>
+        <v>13.476739999999999</v>
       </c>
       <c r="D33" s="1">
-        <v>66.489649999999997</v>
+        <v>66.4465</v>
       </c>
       <c r="E33" s="1">
-        <v>98.43562</v>
+        <v>98.471440000000001</v>
       </c>
       <c r="F33" s="1">
-        <v>4.5407879999999998E-2</v>
+        <v>4.5421040000000003E-2</v>
       </c>
       <c r="G33" s="1">
-        <v>0.99988600000000005</v>
+        <v>0.99988840000000001</v>
       </c>
       <c r="H33" s="1">
-        <v>6.3983150000000003E-2</v>
+        <v>6.4006430000000003E-2</v>
       </c>
       <c r="I33" s="1">
-        <v>1.3688689999999999</v>
+        <v>1.3808180000000001</v>
       </c>
       <c r="J33" s="1">
-        <v>8.2208380000000005</v>
+        <v>8.1749379999999991</v>
       </c>
       <c r="K33" s="1">
-        <v>11.849769999999999</v>
+        <v>11.95989</v>
       </c>
       <c r="L33" s="1">
-        <v>28.13618</v>
+        <v>28.346879999999999</v>
       </c>
       <c r="M33" s="1">
-        <v>8.3848730000000007</v>
+        <v>8.4490700000000007</v>
       </c>
       <c r="N33" s="1">
-        <v>16.71773</v>
+        <v>16.713450000000002</v>
       </c>
       <c r="O33" s="1">
-        <v>999.40549999999996</v>
+        <v>999.40650000000005</v>
       </c>
       <c r="P33" s="1">
         <v>46.887168860000003</v>
@@ -2193,49 +2244,49 @@
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
-        <v>45098.533587962964</v>
+        <v>45098.533599537041</v>
       </c>
       <c r="B34" s="1">
-        <v>9.194502</v>
+        <v>9.1952949999999998</v>
       </c>
       <c r="C34" s="1">
-        <v>13.476739999999999</v>
+        <v>13.479189999999999</v>
       </c>
       <c r="D34" s="1">
-        <v>66.4465</v>
+        <v>66.40334</v>
       </c>
       <c r="E34" s="1">
-        <v>98.471440000000001</v>
+        <v>98.507260000000002</v>
       </c>
       <c r="F34" s="1">
-        <v>4.5421040000000003E-2</v>
+        <v>4.5434189999999999E-2</v>
       </c>
       <c r="G34" s="1">
-        <v>0.99988840000000001</v>
+        <v>0.99989079999999997</v>
       </c>
       <c r="H34" s="1">
-        <v>6.4006430000000003E-2</v>
+        <v>6.4029719999999998E-2</v>
       </c>
       <c r="I34" s="1">
-        <v>1.3808180000000001</v>
+        <v>1.3927670000000001</v>
       </c>
       <c r="J34" s="1">
-        <v>8.1749379999999991</v>
+        <v>8.1290390000000006</v>
       </c>
       <c r="K34" s="1">
-        <v>11.95989</v>
+        <v>12.07001</v>
       </c>
       <c r="L34" s="1">
-        <v>28.346879999999999</v>
+        <v>28.557590000000001</v>
       </c>
       <c r="M34" s="1">
-        <v>8.4490700000000007</v>
+        <v>8.5132670000000008</v>
       </c>
       <c r="N34" s="1">
-        <v>16.713450000000002</v>
+        <v>16.70917</v>
       </c>
       <c r="O34" s="1">
-        <v>999.40650000000005</v>
+        <v>999.40750000000003</v>
       </c>
       <c r="P34" s="1">
         <v>46.887168860000003</v>
@@ -2247,103 +2298,103 @@
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
-        <v>45098.533599537041</v>
+        <v>45098.53361111111</v>
       </c>
       <c r="B35" s="1">
-        <v>9.1952949999999998</v>
+        <v>9.3042200000000008</v>
       </c>
       <c r="C35" s="1">
-        <v>13.479189999999999</v>
+        <v>13.990360000000001</v>
       </c>
       <c r="D35" s="1">
-        <v>66.40334</v>
+        <v>65.834249999999997</v>
       </c>
       <c r="E35" s="1">
-        <v>98.507260000000002</v>
+        <v>98.380330000000001</v>
       </c>
       <c r="F35" s="1">
-        <v>4.5434189999999999E-2</v>
+        <v>4.534266E-2</v>
       </c>
       <c r="G35" s="1">
-        <v>0.99989079999999997</v>
+        <v>0.99990540000000006</v>
       </c>
       <c r="H35" s="1">
-        <v>6.4029719999999998E-2</v>
+        <v>6.3947210000000004E-2</v>
       </c>
       <c r="I35" s="1">
-        <v>1.3927670000000001</v>
+        <v>1.37527</v>
       </c>
       <c r="J35" s="1">
-        <v>8.1290390000000006</v>
+        <v>7.7034539999999998</v>
       </c>
       <c r="K35" s="1">
-        <v>12.07001</v>
+        <v>13.250389999999999</v>
       </c>
       <c r="L35" s="1">
-        <v>28.557590000000001</v>
+        <v>31.245080000000002</v>
       </c>
       <c r="M35" s="1">
-        <v>8.5132670000000008</v>
+        <v>9.3322240000000001</v>
       </c>
       <c r="N35" s="1">
-        <v>16.70917</v>
+        <v>16.692699999999999</v>
       </c>
       <c r="O35" s="1">
-        <v>999.40750000000003</v>
+        <v>999.43409999999994</v>
       </c>
       <c r="P35" s="1">
-        <v>46.887168860000003</v>
+        <v>46.887162170000003</v>
       </c>
       <c r="Q35" s="1">
-        <v>-91.050215499999993</v>
+        <v>-91.050205390000002</v>
       </c>
       <c r="R35" s="1"/>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
-        <v>45098.53361111111</v>
+        <v>45098.533622685187</v>
       </c>
       <c r="B36" s="1">
-        <v>9.3042200000000008</v>
+        <v>9.3058069999999997</v>
       </c>
       <c r="C36" s="1">
-        <v>13.990360000000001</v>
+        <v>14.01801</v>
       </c>
       <c r="D36" s="1">
-        <v>65.834249999999997</v>
+        <v>65.790819999999997</v>
       </c>
       <c r="E36" s="1">
-        <v>98.380330000000001</v>
+        <v>98.382019999999997</v>
       </c>
       <c r="F36" s="1">
-        <v>4.534266E-2</v>
+        <v>4.5340699999999998E-2</v>
       </c>
       <c r="G36" s="1">
-        <v>0.99990540000000006</v>
+        <v>0.99990679999999998</v>
       </c>
       <c r="H36" s="1">
-        <v>6.3947210000000004E-2</v>
+        <v>6.3948309999999994E-2</v>
       </c>
       <c r="I36" s="1">
-        <v>1.37527</v>
+        <v>1.3786959999999999</v>
       </c>
       <c r="J36" s="1">
-        <v>7.7034539999999998</v>
+        <v>7.6745210000000004</v>
       </c>
       <c r="K36" s="1">
-        <v>13.250389999999999</v>
+        <v>13.347020000000001</v>
       </c>
       <c r="L36" s="1">
-        <v>31.245080000000002</v>
+        <v>31.435449999999999</v>
       </c>
       <c r="M36" s="1">
-        <v>9.3322240000000001</v>
+        <v>9.3902140000000003</v>
       </c>
       <c r="N36" s="1">
-        <v>16.692699999999999</v>
+        <v>16.690010000000001</v>
       </c>
       <c r="O36" s="1">
-        <v>999.43409999999994</v>
+        <v>999.43619999999999</v>
       </c>
       <c r="P36" s="1">
         <v>46.887162170000003</v>
@@ -2355,49 +2406,49 @@
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
-        <v>45098.533622685187</v>
+        <v>45098.533634259256</v>
       </c>
       <c r="B37" s="1">
-        <v>9.3058069999999997</v>
+        <v>9.3073949999999996</v>
       </c>
       <c r="C37" s="1">
-        <v>14.01801</v>
+        <v>14.04566</v>
       </c>
       <c r="D37" s="1">
-        <v>65.790819999999997</v>
+        <v>65.747399999999999</v>
       </c>
       <c r="E37" s="1">
-        <v>98.382019999999997</v>
+        <v>98.383709999999994</v>
       </c>
       <c r="F37" s="1">
-        <v>4.5340699999999998E-2</v>
+        <v>4.5338740000000002E-2</v>
       </c>
       <c r="G37" s="1">
-        <v>0.99990679999999998</v>
+        <v>0.99990829999999997</v>
       </c>
       <c r="H37" s="1">
-        <v>6.3948309999999994E-2</v>
+        <v>6.3949409999999998E-2</v>
       </c>
       <c r="I37" s="1">
-        <v>1.3786959999999999</v>
+        <v>1.382123</v>
       </c>
       <c r="J37" s="1">
-        <v>7.6745210000000004</v>
+        <v>7.6455880000000001</v>
       </c>
       <c r="K37" s="1">
-        <v>13.347020000000001</v>
+        <v>13.44364</v>
       </c>
       <c r="L37" s="1">
-        <v>31.435449999999999</v>
+        <v>31.625810000000001</v>
       </c>
       <c r="M37" s="1">
-        <v>9.3902140000000003</v>
+        <v>9.4482040000000005</v>
       </c>
       <c r="N37" s="1">
-        <v>16.690010000000001</v>
+        <v>16.68732</v>
       </c>
       <c r="O37" s="1">
-        <v>999.43619999999999</v>
+        <v>999.43830000000003</v>
       </c>
       <c r="P37" s="1">
         <v>46.887162170000003</v>
@@ -2409,49 +2460,49 @@
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
-        <v>45098.533634259256</v>
+        <v>45098.533645833333</v>
       </c>
       <c r="B38" s="1">
-        <v>9.3073949999999996</v>
+        <v>9.4622679999999999</v>
       </c>
       <c r="C38" s="1">
-        <v>14.04566</v>
+        <v>13.34704</v>
       </c>
       <c r="D38" s="1">
-        <v>65.747399999999999</v>
+        <v>65.368989999999997</v>
       </c>
       <c r="E38" s="1">
-        <v>98.383709999999994</v>
+        <v>98.423879999999997</v>
       </c>
       <c r="F38" s="1">
-        <v>4.5338740000000002E-2</v>
+        <v>4.5260750000000002E-2</v>
       </c>
       <c r="G38" s="1">
-        <v>0.99990829999999997</v>
+        <v>0.99992190000000003</v>
       </c>
       <c r="H38" s="1">
-        <v>6.3949409999999998E-2</v>
+        <v>6.3886709999999999E-2</v>
       </c>
       <c r="I38" s="1">
-        <v>1.382123</v>
+        <v>1.6032569999999999</v>
       </c>
       <c r="J38" s="1">
-        <v>7.6455880000000001</v>
+        <v>7.4243180000000004</v>
       </c>
       <c r="K38" s="1">
-        <v>13.44364</v>
+        <v>14.02955</v>
       </c>
       <c r="L38" s="1">
-        <v>31.625810000000001</v>
+        <v>32.520690000000002</v>
       </c>
       <c r="M38" s="1">
-        <v>9.4482040000000005</v>
+        <v>9.8637530000000009</v>
       </c>
       <c r="N38" s="1">
-        <v>16.68732</v>
+        <v>16.77272</v>
       </c>
       <c r="O38" s="1">
-        <v>999.43830000000003</v>
+        <v>999.42160000000001</v>
       </c>
       <c r="P38" s="1">
         <v>46.887162170000003</v>
@@ -2463,49 +2514,49 @@
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
-        <v>45098.533645833333</v>
+        <v>45098.53365740741</v>
       </c>
       <c r="B39" s="1">
-        <v>9.4622679999999999</v>
+        <v>9.4726169999999996</v>
       </c>
       <c r="C39" s="1">
-        <v>13.34704</v>
+        <v>13.321389999999999</v>
       </c>
       <c r="D39" s="1">
-        <v>65.368989999999997</v>
+        <v>65.337490000000003</v>
       </c>
       <c r="E39" s="1">
-        <v>98.423879999999997</v>
+        <v>98.423640000000006</v>
       </c>
       <c r="F39" s="1">
-        <v>4.5260750000000002E-2</v>
+        <v>4.5254950000000002E-2</v>
       </c>
       <c r="G39" s="1">
-        <v>0.99992190000000003</v>
+        <v>0.99992289999999995</v>
       </c>
       <c r="H39" s="1">
-        <v>6.3886709999999999E-2</v>
+        <v>6.3881960000000002E-2</v>
       </c>
       <c r="I39" s="1">
-        <v>1.6032569999999999</v>
+        <v>1.6143989999999999</v>
       </c>
       <c r="J39" s="1">
-        <v>7.4243180000000004</v>
+        <v>7.4036939999999998</v>
       </c>
       <c r="K39" s="1">
-        <v>14.02955</v>
+        <v>14.084720000000001</v>
       </c>
       <c r="L39" s="1">
-        <v>32.520690000000002</v>
+        <v>32.623730000000002</v>
       </c>
       <c r="M39" s="1">
-        <v>9.8637530000000009</v>
+        <v>9.9025449999999999</v>
       </c>
       <c r="N39" s="1">
-        <v>16.77272</v>
+        <v>16.776789999999998</v>
       </c>
       <c r="O39" s="1">
-        <v>999.42160000000001</v>
+        <v>999.42129999999997</v>
       </c>
       <c r="P39" s="1">
         <v>46.887162170000003</v>
@@ -2517,103 +2568,103 @@
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
-        <v>45098.53365740741</v>
+        <v>45098.533668981479</v>
       </c>
       <c r="B40" s="1">
-        <v>9.4726169999999996</v>
+        <v>9.4829650000000001</v>
       </c>
       <c r="C40" s="1">
-        <v>13.321389999999999</v>
+        <v>13.29574</v>
       </c>
       <c r="D40" s="1">
-        <v>65.337490000000003</v>
+        <v>65.305980000000005</v>
       </c>
       <c r="E40" s="1">
-        <v>98.423640000000006</v>
+        <v>98.423389999999998</v>
       </c>
       <c r="F40" s="1">
-        <v>4.5254950000000002E-2</v>
+        <v>4.5249150000000002E-2</v>
       </c>
       <c r="G40" s="1">
-        <v>0.99992289999999995</v>
+        <v>0.99992389999999998</v>
       </c>
       <c r="H40" s="1">
-        <v>6.3881960000000002E-2</v>
+        <v>6.3877199999999995E-2</v>
       </c>
       <c r="I40" s="1">
-        <v>1.6143989999999999</v>
+        <v>1.62554</v>
       </c>
       <c r="J40" s="1">
-        <v>7.4036939999999998</v>
+        <v>7.38307</v>
       </c>
       <c r="K40" s="1">
-        <v>14.084720000000001</v>
+        <v>14.139900000000001</v>
       </c>
       <c r="L40" s="1">
-        <v>32.623730000000002</v>
+        <v>32.726770000000002</v>
       </c>
       <c r="M40" s="1">
-        <v>9.9025449999999999</v>
+        <v>9.9413359999999997</v>
       </c>
       <c r="N40" s="1">
-        <v>16.776789999999998</v>
+        <v>16.780860000000001</v>
       </c>
       <c r="O40" s="1">
-        <v>999.42129999999997</v>
+        <v>999.42100000000005</v>
       </c>
       <c r="P40" s="1">
-        <v>46.887162170000003</v>
+        <v>46.887153849999997</v>
       </c>
       <c r="Q40" s="1">
-        <v>-91.050205390000002</v>
+        <v>-91.050198249999994</v>
       </c>
       <c r="R40" s="1"/>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
-        <v>45098.533668981479</v>
+        <v>45098.533680555556</v>
       </c>
       <c r="B41" s="1">
-        <v>9.4829650000000001</v>
+        <v>10.892519999999999</v>
       </c>
       <c r="C41" s="1">
-        <v>13.29574</v>
+        <v>13.12153</v>
       </c>
       <c r="D41" s="1">
-        <v>65.305980000000005</v>
+        <v>65.236930000000001</v>
       </c>
       <c r="E41" s="1">
-        <v>98.423389999999998</v>
+        <v>98.471080000000001</v>
       </c>
       <c r="F41" s="1">
-        <v>4.5249150000000002E-2</v>
+        <v>4.5332740000000003E-2</v>
       </c>
       <c r="G41" s="1">
-        <v>0.99992389999999998</v>
+        <v>0.9999247</v>
       </c>
       <c r="H41" s="1">
-        <v>6.3877199999999995E-2</v>
+        <v>6.3993419999999995E-2</v>
       </c>
       <c r="I41" s="1">
-        <v>1.62554</v>
+        <v>2.974618</v>
       </c>
       <c r="J41" s="1">
-        <v>7.38307</v>
+        <v>7.3373999999999997</v>
       </c>
       <c r="K41" s="1">
-        <v>14.139900000000001</v>
+        <v>14.10186</v>
       </c>
       <c r="L41" s="1">
-        <v>32.726770000000002</v>
+        <v>32.596899999999998</v>
       </c>
       <c r="M41" s="1">
-        <v>9.9413359999999997</v>
+        <v>9.9145939999999992</v>
       </c>
       <c r="N41" s="1">
-        <v>16.780860000000001</v>
+        <v>16.820709999999998</v>
       </c>
       <c r="O41" s="1">
-        <v>999.42100000000005</v>
+        <v>999.3954</v>
       </c>
       <c r="P41" s="1">
         <v>46.887153849999997</v>
@@ -2625,49 +2676,49 @@
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
-        <v>45098.533680555556</v>
+        <v>45098.533692129633</v>
       </c>
       <c r="B42" s="1">
-        <v>10.892519999999999</v>
+        <v>10.968400000000001</v>
       </c>
       <c r="C42" s="1">
-        <v>13.12153</v>
+        <v>13.09775</v>
       </c>
       <c r="D42" s="1">
-        <v>65.236930000000001</v>
+        <v>65.225589999999997</v>
       </c>
       <c r="E42" s="1">
-        <v>98.471080000000001</v>
+        <v>98.474490000000003</v>
       </c>
       <c r="F42" s="1">
-        <v>4.5332740000000003E-2</v>
+        <v>4.5335489999999999E-2</v>
       </c>
       <c r="G42" s="1">
-        <v>0.9999247</v>
+        <v>0.99992499999999995</v>
       </c>
       <c r="H42" s="1">
-        <v>6.3993419999999995E-2</v>
+        <v>6.3998180000000002E-2</v>
       </c>
       <c r="I42" s="1">
-        <v>2.974618</v>
+        <v>3.0488919999999999</v>
       </c>
       <c r="J42" s="1">
-        <v>7.3373999999999997</v>
+        <v>7.3305600000000002</v>
       </c>
       <c r="K42" s="1">
-        <v>14.10186</v>
+        <v>14.11191</v>
       </c>
       <c r="L42" s="1">
-        <v>32.596899999999998</v>
+        <v>32.608130000000003</v>
       </c>
       <c r="M42" s="1">
-        <v>9.9145939999999992</v>
+        <v>9.9216610000000003</v>
       </c>
       <c r="N42" s="1">
-        <v>16.820709999999998</v>
+        <v>16.824539999999999</v>
       </c>
       <c r="O42" s="1">
-        <v>999.3954</v>
+        <v>999.39369999999997</v>
       </c>
       <c r="P42" s="1">
         <v>46.887153849999997</v>
@@ -2679,49 +2730,49 @@
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
-        <v>45098.533692129633</v>
+        <v>45098.533703703702</v>
       </c>
       <c r="B43" s="1">
-        <v>10.968400000000001</v>
+        <v>11.04429</v>
       </c>
       <c r="C43" s="1">
-        <v>13.09775</v>
+        <v>13.073969999999999</v>
       </c>
       <c r="D43" s="1">
-        <v>65.225589999999997</v>
+        <v>65.214259999999996</v>
       </c>
       <c r="E43" s="1">
-        <v>98.474490000000003</v>
+        <v>98.477900000000005</v>
       </c>
       <c r="F43" s="1">
-        <v>4.5335489999999999E-2</v>
+        <v>4.533823E-2</v>
       </c>
       <c r="G43" s="1">
-        <v>0.99992499999999995</v>
+        <v>0.99992539999999996</v>
       </c>
       <c r="H43" s="1">
-        <v>6.3998180000000002E-2</v>
+        <v>6.4002939999999994E-2</v>
       </c>
       <c r="I43" s="1">
-        <v>3.0488919999999999</v>
+        <v>3.1231659999999999</v>
       </c>
       <c r="J43" s="1">
-        <v>7.3305600000000002</v>
+        <v>7.3237199999999998</v>
       </c>
       <c r="K43" s="1">
-        <v>14.11191</v>
+        <v>14.12196</v>
       </c>
       <c r="L43" s="1">
-        <v>32.608130000000003</v>
+        <v>32.61936</v>
       </c>
       <c r="M43" s="1">
-        <v>9.9216610000000003</v>
+        <v>9.9287290000000006</v>
       </c>
       <c r="N43" s="1">
-        <v>16.824539999999999</v>
+        <v>16.82837</v>
       </c>
       <c r="O43" s="1">
-        <v>999.39369999999997</v>
+        <v>999.39200000000005</v>
       </c>
       <c r="P43" s="1">
         <v>46.887153849999997</v>
@@ -2733,49 +2784,49 @@
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
-        <v>45098.533703703702</v>
+        <v>45098.533715277779</v>
       </c>
       <c r="B44" s="1">
-        <v>11.04429</v>
+        <v>24.51182</v>
       </c>
       <c r="C44" s="1">
-        <v>13.073969999999999</v>
+        <v>12.91292</v>
       </c>
       <c r="D44" s="1">
-        <v>65.214259999999996</v>
+        <v>65.243319999999997</v>
       </c>
       <c r="E44" s="1">
-        <v>98.477900000000005</v>
+        <v>98.414490000000001</v>
       </c>
       <c r="F44" s="1">
-        <v>4.533823E-2</v>
+        <v>4.531541E-2</v>
       </c>
       <c r="G44" s="1">
-        <v>0.99992539999999996</v>
+        <v>0.99992329999999996</v>
       </c>
       <c r="H44" s="1">
-        <v>6.4002939999999994E-2</v>
+        <v>6.3961710000000005E-2</v>
       </c>
       <c r="I44" s="1">
-        <v>3.1231659999999999</v>
+        <v>3.0222690000000001</v>
       </c>
       <c r="J44" s="1">
-        <v>7.3237199999999998</v>
+        <v>7.3541280000000002</v>
       </c>
       <c r="K44" s="1">
-        <v>14.12196</v>
+        <v>14.14373</v>
       </c>
       <c r="L44" s="1">
-        <v>32.61936</v>
+        <v>32.66968</v>
       </c>
       <c r="M44" s="1">
-        <v>9.9287290000000006</v>
+        <v>9.9440329999999992</v>
       </c>
       <c r="N44" s="1">
-        <v>16.82837</v>
+        <v>16.707439999999998</v>
       </c>
       <c r="O44" s="1">
-        <v>999.39200000000005</v>
+        <v>999.39940000000001</v>
       </c>
       <c r="P44" s="1">
         <v>46.887153849999997</v>
@@ -2787,84 +2838,30 @@
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
-        <v>45098.533715277779</v>
+        <v>45098.533726851849</v>
       </c>
       <c r="B45" s="1">
-        <v>24.51182</v>
+        <v>25.276119999999999</v>
       </c>
       <c r="C45" s="1">
-        <v>12.91292</v>
+        <v>12.901120000000001</v>
       </c>
       <c r="D45" s="1">
-        <v>65.243319999999997</v>
+        <v>65.243759999999995</v>
       </c>
       <c r="E45" s="1">
-        <v>98.414490000000001</v>
+        <v>98.411940000000001</v>
       </c>
       <c r="F45" s="1">
-        <v>4.531541E-2</v>
+        <v>4.5315870000000001E-2</v>
       </c>
       <c r="G45" s="1">
-        <v>0.99992329999999996</v>
+        <v>0.99992320000000001</v>
       </c>
       <c r="H45" s="1">
-        <v>6.3961710000000005E-2</v>
+        <v>6.3961809999999994E-2</v>
       </c>
       <c r="I45" s="1">
-        <v>3.0222690000000001</v>
-      </c>
-      <c r="J45" s="1">
-        <v>7.3541280000000002</v>
-      </c>
-      <c r="K45" s="1">
-        <v>14.14373</v>
-      </c>
-      <c r="L45" s="1">
-        <v>32.66968</v>
-      </c>
-      <c r="M45" s="1">
-        <v>9.9440329999999992</v>
-      </c>
-      <c r="N45" s="1">
-        <v>16.707439999999998</v>
-      </c>
-      <c r="O45" s="1">
-        <v>999.39940000000001</v>
-      </c>
-      <c r="P45" s="1">
-        <v>46.887153849999997</v>
-      </c>
-      <c r="Q45" s="1">
-        <v>-91.050198249999994</v>
-      </c>
-      <c r="R45" s="1"/>
-    </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A46" s="2">
-        <v>45098.533726851849</v>
-      </c>
-      <c r="B46" s="1">
-        <v>25.276119999999999</v>
-      </c>
-      <c r="C46" s="1">
-        <v>12.901120000000001</v>
-      </c>
-      <c r="D46" s="1">
-        <v>65.243759999999995</v>
-      </c>
-      <c r="E46" s="1">
-        <v>98.411940000000001</v>
-      </c>
-      <c r="F46" s="1">
-        <v>4.5315870000000001E-2</v>
-      </c>
-      <c r="G46" s="1">
-        <v>0.99992320000000001</v>
-      </c>
-      <c r="H46" s="1">
-        <v>6.3961809999999994E-2</v>
-      </c>
-      <c r="I46" s="1">
         <v>3.0434169999999998</v>
       </c>
     </row>

</xml_diff>